<commit_message>
Update results for ArDoCo
</commit_message>
<xml_diff>
--- a/results/ArDoCo.xlsx
+++ b/results/ArDoCo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan Keim\Projects\Repos\ArDoCo\ReplicationPackageICSE24\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F23553-8ED7-427B-91A9-88B8D7EE102D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9272C99C-8809-4A0A-99A0-668876D1A799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13695" yWindow="0" windowWidth="28800" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9180" yWindow="345" windowWidth="28800" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAD-SAM-Code" sheetId="3" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,7 @@
         <v>0.61</v>
       </c>
       <c r="D6" s="1">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="E6" s="1">
         <v>0.74</v>
@@ -608,7 +608,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" ref="D9:H9" si="0">SUM(D4:D8)/COUNT(D4:D8)</f>
-        <v>0.81799999999999995</v>
+        <v>0.81600000000000006</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
@@ -637,7 +637,7 @@
       </c>
       <c r="D10" s="1">
         <f>(D4*Projects!$C$4+D5*Projects!$C$5+D6*Projects!$C$6+D7*Projects!$C$7+D8*Projects!$C$8)/SUM(Projects!$C$4:$C$8)</f>
-        <v>0.96074494025847357</v>
+        <v>0.95694708607656676</v>
       </c>
       <c r="E10" s="1">
         <f>(E4*Projects!$C$4+E5*Projects!$C$5+E6*Projects!$C$6+E7*Projects!$C$7+E8*Projects!$C$8)/SUM(Projects!$C$4:$C$8)</f>

</xml_diff>

<commit_message>
Add evaluator and scripts
</commit_message>
<xml_diff>
--- a/results/ArDoCo.xlsx
+++ b/results/ArDoCo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan Keim\Projects\Repos\ArDoCo\ReplicationPackageICSE24\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9272C99C-8809-4A0A-99A0-668876D1A799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E8EFCC-19E5-4BB1-842B-85BA631E5D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="345" windowWidth="28800" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13695" yWindow="0" windowWidth="28800" windowHeight="15585" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAD-SAM-Code" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
   <si>
     <t>Project</t>
   </si>
@@ -86,13 +86,16 @@
     <t>Number of Trace Links in Gold Standard</t>
   </si>
   <si>
-    <t>SAD-SAM-Code</t>
-  </si>
-  <si>
     <t>SAD-SAM</t>
   </si>
   <si>
     <t>SAM-Code</t>
+  </si>
+  <si>
+    <t>Confusion matrix sums</t>
+  </si>
+  <si>
+    <t>SAD-Code</t>
   </si>
 </sst>
 </file>
@@ -446,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C95C70-6BB0-4836-8225-CF2F6DDCE834}">
   <dimension ref="B3:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1092,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E94EC2-DE1C-4D94-82AD-DEE5FCED1B3C}">
-  <dimension ref="B2:E8"/>
+  <dimension ref="B2:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,13 +1117,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1191,6 +1194,95 @@
       </c>
       <c r="E8">
         <v>1956</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>3589</v>
+      </c>
+      <c r="D13">
+        <v>518</v>
+      </c>
+      <c r="E13">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>8815</v>
+      </c>
+      <c r="D14">
+        <v>473</v>
+      </c>
+      <c r="E14">
+        <v>3895</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>165330</v>
+      </c>
+      <c r="D15">
+        <v>1584</v>
+      </c>
+      <c r="E15">
+        <v>13360</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>47600</v>
+      </c>
+      <c r="D16">
+        <v>1020</v>
+      </c>
+      <c r="E16">
+        <v>13440</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>26000</v>
+      </c>
+      <c r="D17">
+        <v>78</v>
+      </c>
+      <c r="E17">
+        <v>12000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update gold standards & update results for ArDoCo
</commit_message>
<xml_diff>
--- a/results/ArDoCo.xlsx
+++ b/results/ArDoCo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan Keim\Projects\Repos\ArDoCo\ReplicationPackageICSE24\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominik\Projects\Paper\2023\icse-2024\ReplicationPackageICSE24\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3877777F-56CC-4F5C-813D-1775D5006685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBC9288-F261-44E2-A0AF-C48425732BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="1200" windowWidth="28680" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAD-Code" sheetId="3" r:id="rId1"/>
@@ -191,7 +191,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -472,20 +472,20 @@
   <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.1796875" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -508,18 +508,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
       <c r="D4" s="1">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="E4" s="1">
-        <v>0.83</v>
+        <v>0.84</v>
       </c>
       <c r="F4" s="1">
         <v>0.99</v>
@@ -531,7 +531,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
@@ -554,7 +554,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -577,7 +577,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -600,7 +600,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -623,21 +623,21 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1">
         <f>SUM(C4:C8)/COUNT(C4:C8)</f>
-        <v>0.87199999999999989</v>
+        <v>0.874</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" ref="D9:H9" si="0">SUM(D4:D8)/COUNT(D4:D8)</f>
-        <v>0.81200000000000006</v>
+        <v>0.81000000000000016</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>0.81600000000000006</v>
+        <v>0.81799999999999995</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
@@ -652,33 +652,33 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1">
         <f>(C6*Projects!$C$6+C8*Projects!$C$8+C7*Projects!$C$7+C4*Projects!$C$4+C5*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
-        <v>0.80885226702359037</v>
+        <v>0.80918548787895528</v>
       </c>
       <c r="D10" s="1">
         <f>(D6*Projects!$C$6+D8*Projects!$C$8+D7*Projects!$C$7+D4*Projects!$C$4+D5*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
-        <v>0.94324800624616589</v>
+        <v>0.94220608537191453</v>
       </c>
       <c r="E10" s="1">
         <f>(E6*Projects!$C$6+E8*Projects!$C$8+E7*Projects!$C$7+E4*Projects!$C$4+E5*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
-        <v>0.86756901455579727</v>
+        <v>0.86801314263625817</v>
       </c>
       <c r="F10" s="1">
         <f>(F6*Projects!$C$6+F8*Projects!$C$8+F7*Projects!$C$7+F4*Projects!$C$4+F5*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
-        <v>0.97152807986169187</v>
+        <v>0.97170964713678276</v>
       </c>
       <c r="G10" s="1">
         <f>(G6*Projects!$C$6+G8*Projects!$C$8+G7*Projects!$C$7+G4*Projects!$C$4+G5*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
-        <v>0.96312252523562525</v>
+        <v>0.96338671378872365</v>
       </c>
       <c r="H10" s="1">
         <f>(H6*Projects!$C$6+H8*Projects!$C$8+H7*Projects!$C$7+H4*Projects!$C$4+H5*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
-        <v>0.85421393118063693</v>
+        <v>0.85397592357391361</v>
       </c>
     </row>
   </sheetData>
@@ -691,16 +691,16 @@
   <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -723,7 +723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
@@ -746,7 +746,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
@@ -769,7 +769,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -792,7 +792,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -815,7 +815,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -838,7 +838,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
@@ -867,7 +867,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
@@ -906,15 +906,15 @@
   <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -937,30 +937,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>0.87</v>
+        <v>0.94</v>
       </c>
       <c r="D4" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="E4" s="1">
         <v>0.95</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.91</v>
       </c>
       <c r="F4" s="1">
         <v>0.99</v>
       </c>
       <c r="G4" s="1">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
@@ -983,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1052,21 +1052,21 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1">
         <f>SUM(C4:C8)/COUNT(C4:C8)</f>
-        <v>0.96599999999999997</v>
+        <v>0.98000000000000009</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" ref="D9:H9" si="0">SUM(D4:D8)/COUNT(D4:D8)</f>
-        <v>0.98599999999999999</v>
+        <v>0.98799999999999988</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>0.9760000000000002</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
@@ -1074,40 +1074,40 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.998</v>
+        <v>1</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
-        <v>0.97399999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.98199999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1">
         <f>(C6*Projects!$E$6+C8*Projects!$E$8+C7*Projects!$E$7+C4*Projects!$E$4+C5*Projects!$E$5)/SUM(Projects!$E$4:$E$8)</f>
-        <v>0.97910307898259707</v>
+        <v>0.98933274414494021</v>
       </c>
       <c r="D10" s="1">
         <f>(D6*Projects!$E$6+D8*Projects!$E$8+D7*Projects!$E$7+D4*Projects!$E$4+D5*Projects!$E$5)/SUM(Projects!$E$4:$E$8)</f>
-        <v>0.9916153502900491</v>
+        <v>0.99282368537339827</v>
       </c>
       <c r="E10" s="1">
         <f>(E6*Projects!$E$6+E8*Projects!$E$8+E7*Projects!$E$7+E4*Projects!$E$4+E5*Projects!$E$5)/SUM(Projects!$E$4:$E$8)</f>
-        <v>0.98535921463632314</v>
+        <v>0.99107821475916924</v>
       </c>
       <c r="F10" s="1">
         <f>(F6*Projects!$E$6+F8*Projects!$E$8+F7*Projects!$E$7+F4*Projects!$E$4+F5*Projects!$E$5)/SUM(Projects!$E$4:$E$8)</f>
-        <v>0.9984694332887103</v>
+        <v>0.99838709677419346</v>
       </c>
       <c r="G10" s="1">
         <f>(G6*Projects!$E$6+G8*Projects!$E$8+G7*Projects!$E$7+G4*Projects!$E$4+G5*Projects!$E$5)/SUM(Projects!$E$4:$E$8)</f>
-        <v>0.9984694332887103</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1">
         <f>(H6*Projects!$E$6+H8*Projects!$E$8+H7*Projects!$E$7+H4*Projects!$E$4+H5*Projects!$E$5)/SUM(Projects!$E$4:$E$8)</f>
-        <v>0.98499330655957162</v>
+        <v>0.99071586389748112</v>
       </c>
     </row>
   </sheetData>
@@ -1120,21 +1120,21 @@
   <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1148,21 +1148,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4">
-        <v>1295</v>
+        <v>1473</v>
       </c>
       <c r="D4">
         <v>52</v>
       </c>
       <c r="E4">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -1218,12 +1218,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>13440</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>2231</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>13360</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Add results for direct TLs to ArDoCo.xlsx
</commit_message>
<xml_diff>
--- a/results/ArDoCo.xlsx
+++ b/results/ArDoCo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominik\Projects\Paper\2023\icse-2024\ReplicationPackageICSE24\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBC9288-F261-44E2-A0AF-C48425732BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EF1B74-85D5-4564-A52E-2E62C3BA7DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="1200" windowWidth="28680" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="2010" windowWidth="28670" windowHeight="15320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAD-Code" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="20">
   <si>
     <t>Project</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Confusion matrix sums / Solution Space Size</t>
+  </si>
+  <si>
+    <t>Transitive</t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C95C70-6BB0-4836-8225-CF2F6DDCE834}">
-  <dimension ref="B3:H10"/>
+  <dimension ref="A2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,7 +488,12 @@
     <col min="8" max="8" width="8.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -508,7 +516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
@@ -531,7 +539,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
@@ -554,7 +562,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -577,7 +585,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -600,7 +608,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -623,7 +631,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
@@ -652,7 +660,7 @@
         <v>0.81799999999999995</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
@@ -679,6 +687,202 @@
       <c r="H10" s="1">
         <f>(H6*Projects!$C$6+H8*Projects!$C$8+H7*Projects!$C$7+H4*Projects!$C$4+H5*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
         <v>0.85397592357391361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
+        <f>SUM(C14:C18)/COUNT(C14:C18)</f>
+        <v>0.26</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" ref="D19:H19" si="1">SUM(D14:D18)/COUNT(D14:D18)</f>
+        <v>0.78</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.372</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.81199999999999994</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79399999999999993</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.35599999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="1">
+        <f>(C16*Projects!$C$6+C18*Projects!$C$8+C17*Projects!$C$7+C14*Projects!$C$4+C15*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
+        <v>0.44801645590590317</v>
+      </c>
+      <c r="D20" s="1">
+        <f>(D16*Projects!$C$6+D18*Projects!$C$8+D17*Projects!$C$7+D14*Projects!$C$4+D15*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
+        <v>0.92451377767960685</v>
+      </c>
+      <c r="E20" s="1">
+        <f>(E16*Projects!$C$6+E18*Projects!$C$8+E17*Projects!$C$7+E14*Projects!$C$4+E15*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
+        <v>0.60948202551217634</v>
+      </c>
+      <c r="F20" s="1">
+        <f>(F16*Projects!$C$6+F18*Projects!$C$8+F17*Projects!$C$7+F14*Projects!$C$4+F15*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
+        <v>0.84652051466121814</v>
+      </c>
+      <c r="G20" s="1">
+        <f>(G16*Projects!$C$6+G18*Projects!$C$8+G17*Projects!$C$7+G14*Projects!$C$4+G15*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
+        <v>0.80585233861615768</v>
+      </c>
+      <c r="H20" s="1">
+        <f>(H16*Projects!$C$6+H18*Projects!$C$8+H17*Projects!$C$7+H14*Projects!$C$4+H15*Projects!$C$5)/SUM(Projects!$C$4:$C$8)</f>
+        <v>0.55522723507648131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>